<commit_message>
modify codes of multi neural network and apply it to smaller sized dataset
</commit_message>
<xml_diff>
--- a/result/rating_experiments.xlsx
+++ b/result/rating_experiments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Exp1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,11 @@
     <sheet name="Exp5" sheetId="5" r:id="rId5"/>
     <sheet name="userNN" sheetId="6" r:id="rId6"/>
     <sheet name="MF" sheetId="7" r:id="rId7"/>
+    <sheet name="Exp6" sheetId="8" r:id="rId8"/>
+    <sheet name="Exp7" sheetId="9" r:id="rId9"/>
+    <sheet name="Exp8" sheetId="10" r:id="rId10"/>
+    <sheet name="Exp9" sheetId="11" r:id="rId11"/>
+    <sheet name="MNN" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="54">
   <si>
     <t>/Users/Jerry/anaconda/bin/python /Users/Jerry/Documents/project_learning/RecommenderSystemPython/model/benchmark_of_rating_predictors.py</t>
   </si>
@@ -156,6 +161,45 @@
   </si>
   <si>
     <t>Number of  Latent Factor</t>
+  </si>
+  <si>
+    <t>Test new model MultiNeuralNetwork:</t>
+  </si>
+  <si>
+    <t>threshold number of observed ratings: 2</t>
+  </si>
+  <si>
+    <t>[1.0226522566515115, 1.1036317675451726, 1.0796453438104525, 1.0268363468129409, 1.1111794707803886]</t>
+  </si>
+  <si>
+    <t>1.06878903712 0.0374631948994</t>
+  </si>
+  <si>
+    <t>threshold number of observed ratings: 5</t>
+  </si>
+  <si>
+    <t>[1.0849279885217245, 1.1048108294254293, 1.0622359042419014, 0.9922596866745812, 1.0947759969686426]</t>
+  </si>
+  <si>
+    <t>1.06780208117 0.0403191566759</t>
+  </si>
+  <si>
+    <t>threshold number of observed ratings: 10</t>
+  </si>
+  <si>
+    <t>[0.83133108992501203, 0.83436182511790713, 0.82994877744839335, 0.83171960931433087, 0.84673072685773498]</t>
+  </si>
+  <si>
+    <t>0.834818405733 0.00612517837873</t>
+  </si>
+  <si>
+    <t>threshold number of observed ratings: 8</t>
+  </si>
+  <si>
+    <t>[1.1467991727635307, 1.2420360291408481, 0.82994877744839335, 1.2584760261689947, 1.4091918148254987]</t>
+  </si>
+  <si>
+    <t>1.17729036407 0.192944181712</t>
   </si>
 </sst>
 </file>
@@ -593,11 +637,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="2098230448"/>
-        <c:axId val="-2066561040"/>
+        <c:axId val="-2087293840"/>
+        <c:axId val="-2106343008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2098230448"/>
+        <c:axId val="-2087293840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -637,7 +681,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2066561040"/>
+        <c:crossAx val="-2106343008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -645,7 +689,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2066561040"/>
+        <c:axId val="-2106343008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -681,7 +725,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2098230448"/>
+        <c:crossAx val="-2087293840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1104,11 +1148,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-1986973936"/>
-        <c:axId val="-1981950704"/>
+        <c:axId val="-2071207312"/>
+        <c:axId val="-2071203904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1986973936"/>
+        <c:axId val="-2071207312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1148,7 +1192,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1981950704"/>
+        <c:crossAx val="-2071203904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1156,7 +1200,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1981950704"/>
+        <c:axId val="-2071203904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1189,7 +1233,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1986973936"/>
+        <c:crossAx val="-2071207312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2728,6 +2772,197 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.84673072685799999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1.40919181483</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
@@ -3448,8 +3683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3517,4 +3752,164 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1.11117947078</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1.0947759969699999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update data and experiment settings
</commit_message>
<xml_diff>
--- a/result/rating_experiments.xlsx
+++ b/result/rating_experiments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="11"/>
+    <workbookView xWindow="13400" yWindow="2140" windowWidth="21820" windowHeight="15300" tabRatio="500" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Exp1" sheetId="1" r:id="rId1"/>
@@ -169,37 +169,37 @@
     <t>threshold number of observed ratings: 2</t>
   </si>
   <si>
-    <t>[1.0226522566515115, 1.1036317675451726, 1.0796453438104525, 1.0268363468129409, 1.1111794707803886]</t>
-  </si>
-  <si>
-    <t>1.06878903712 0.0374631948994</t>
-  </si>
-  <si>
     <t>threshold number of observed ratings: 5</t>
   </si>
   <si>
-    <t>[1.0849279885217245, 1.1048108294254293, 1.0622359042419014, 0.9922596866745812, 1.0947759969686426]</t>
-  </si>
-  <si>
-    <t>1.06780208117 0.0403191566759</t>
-  </si>
-  <si>
     <t>threshold number of observed ratings: 10</t>
   </si>
   <si>
-    <t>[0.83133108992501203, 0.83436182511790713, 0.82994877744839335, 0.83171960931433087, 0.84673072685773498]</t>
-  </si>
-  <si>
-    <t>0.834818405733 0.00612517837873</t>
-  </si>
-  <si>
     <t>threshold number of observed ratings: 8</t>
   </si>
   <si>
-    <t>[1.1467991727635307, 1.2420360291408481, 0.82994877744839335, 1.2584760261689947, 1.4091918148254987]</t>
-  </si>
-  <si>
-    <t>1.17729036407 0.192944181712</t>
+    <t>[1.0924824749807964, 1.1051300566259838, 1.1226575764489921, 1.1115644687001511, 1.2494529716767813]</t>
+  </si>
+  <si>
+    <t>1.13625750969 0.0574335948203</t>
+  </si>
+  <si>
+    <t>[1.1039037860610217, 1.1612489498001699, 1.2495518234516396, 1.1838002807216113, 1.2473442901233411]</t>
+  </si>
+  <si>
+    <t>1.18916982603 0.0549708264508</t>
+  </si>
+  <si>
+    <t>[1.084718628978713, 1.1397237076056712, 0.90561248963661911, 1.3588210480366205, 1.406481708133454]</t>
+  </si>
+  <si>
+    <t>1.17907151648 0.183986872449</t>
+  </si>
+  <si>
+    <t>[0.9406605241530368, 0.90003271502768523, 0.90561248963661911, 1.0313874267786003, 0.94245801594933409]</t>
+  </si>
+  <si>
+    <t>0.944030234309 0.0470251224388</t>
   </si>
 </sst>
 </file>
@@ -318,6 +318,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -445,6 +446,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -566,6 +568,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -741,6 +744,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1308,6 +1312,521 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>Root Mean Square</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+              <a:t> Error vs Rating Size Threshold</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2000"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MNN!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RMSE_test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>MNN!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>@</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MNN!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.1223137</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.16758411</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.31889086</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.846730726858</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MNN!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RMSE_train</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>MNN!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>@</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MNN!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.13625750969</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.189169826</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.17907151648</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9440302343</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="-2080775120"/>
+        <c:axId val="-2080849952"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2080775120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="@" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2080849952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2080849952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2080775120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1388,6 +1907,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
   <cs:axisTitle>
@@ -1858,6 +2417,475 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2375,6 +3403,41 @@
       <xdr:colOff>482600</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2777,7 +3840,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B18"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2799,7 +3862,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2829,17 +3892,17 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>0.84673072685799999</v>
+        <v>1.3188908615099999</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -2857,7 +3920,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2879,7 +3942,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2919,7 +3982,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1.40919181483</v>
+        <v>0.84673072685799999</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -2934,15 +3997,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2958,8 +4021,53 @@
         <v>39</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.1223137000000001</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.1362575096900001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.16758411</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.1891698260000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.31889086</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.1790715164800001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.84673072685799999</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.94403023429999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3759,7 +4867,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3811,17 +4919,17 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1.11117947078</v>
+        <v>1.1223137003000001</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -3839,7 +4947,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3861,7 +4969,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3891,17 +4999,17 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1.0947759969699999</v>
+        <v>1.1675841149499999</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>